<commit_message>
(almost) fixed no-username reg
</commit_message>
<xml_diff>
--- a/ValoShop/users.xlsx
+++ b/ValoShop/users.xlsx
@@ -394,7 +394,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C5"/>
@@ -440,7 +440,41 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Константин2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2К</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>26.2.2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>qiviCHAN3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>3q</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>26.2.2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="5"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -452,7 +486,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
@@ -654,6 +688,200 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2К</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ke0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>сс0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>sy0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>fy0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>gt0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>sf0</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>by0</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>ml0</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>sr0</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>as0</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>se0</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>je0</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>bg0</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>gn0</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>pm0</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>vl0</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>on0</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>or0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3q</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ke0</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>сс0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>sy0</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>fy0</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>gt0</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>sf0</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>by0</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>ml0</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>sr0</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>as0</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>se0</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>je0</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>bg0</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>gn0</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>pm0</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>vl0</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>on0</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>or0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
FINALLY fixed no-username registration
bozhe kak zhe ya zaebalsya
</commit_message>
<xml_diff>
--- a/ValoShop/users.xlsx
+++ b/ValoShop/users.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A7" sqref="A2:C7"/>
+      <selection activeCell="A6" sqref="A2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -427,7 +427,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Константин1</t>
+          <t>magnitgd</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -453,7 +453,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A15" sqref="A2:S15"/>
+      <selection activeCell="A17" sqref="A2:S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>

</xml_diff>